<commit_message>
fine ZSS-1035 test case
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/issue/book/1035-repeat-column-titles-pdf.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/issue/book/1035-repeat-column-titles-pdf.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
   <si>
     <t>As Of:</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>CURRENT</t>
+  </si>
+  <si>
+    <t>repeat Column A:C</t>
   </si>
 </sst>
 </file>
@@ -81,9 +84,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_-&quot;NT$&quot;* #,##0.00_-;\-&quot;NT$&quot;* #,##0.00_-;_-&quot;NT$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;NT$&quot;* #,##0.00_-;\-&quot;NT$&quot;* #,##0.00_-;_-&quot;NT$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -180,22 +183,22 @@
   </borders>
   <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -209,17 +212,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -234,7 +237,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -596,7 +599,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1"/>
@@ -616,7 +619,9 @@
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1"/>
+      <c r="B1" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="C1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
@@ -632,9 +637,8 @@
       </c>
       <c r="B2" s="7">
         <f ca="1">NOW()</f>
-        <v>42122.445022222222</v>
-      </c>
-      <c r="C2" s="8"/>
+        <v>42123.487560995367</v>
+      </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>

</xml_diff>